<commit_message>
complete draft for DU Template 1 and 2
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_PREGNANCY-COHORT_variables.xlsx
+++ b/i_codebooks/D3_DU_PREGNANCY-COHORT_variables.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="145">
   <si>
     <t>medatata_name</t>
   </si>
@@ -179,18 +179,9 @@
     <t>Whether woman has MS during this pregnancy</t>
   </si>
   <si>
-    <t>Whether woman has MS ever</t>
-  </si>
-  <si>
     <t>exit from the SAP1 study</t>
   </si>
   <si>
-    <t>this is missing for all pregnancies where the linkage with D3_DU_MS-COHORT fails</t>
-  </si>
-  <si>
-    <t>D3_DU_MS-COHORT</t>
-  </si>
-  <si>
     <t xml:space="preserve"> is non-missing</t>
   </si>
   <si>
@@ -213,16 +204,6 @@
   </si>
   <si>
     <t>int</t>
-  </si>
-  <si>
-    <t>See Figure 3 of the SAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"no" = no MS ever during the pregnancy
-"during pregnancy" = MS diagnosed between pregnancy_start_date and DU_pregnancy_study_exit_date
-"right before pregnancy" = MS diagnosed between DU_pregnancy_study_entry_date and pregnancy_start_date
-"before pregnancy" = MS diagnosed before DU_pregnancy_study_entry_date
-</t>
   </si>
   <si>
     <t>D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY-COHORT</t>
@@ -247,50 +228,257 @@
     <t xml:space="preserve">int </t>
   </si>
   <si>
-    <t>1 = pregnancy_with_MS_detail == "before  pregnancy"
+    <t>number of pregnancies with pregnancy_with_MS == 1</t>
+  </si>
+  <si>
+    <t>this is missing if has_MS_ever == 0, and 0 if has_MS_ever == 1 but there are no pregnancies with pregnancy_with_MS == 1</t>
+  </si>
+  <si>
+    <t>time_since_previous_pregnancy</t>
+  </si>
+  <si>
+    <t>has_previous_pregnancy</t>
+  </si>
+  <si>
+    <t>whether this pregnancy has a previous pregnancy of the same person in the study</t>
+  </si>
+  <si>
+    <t>missing if has_previous_pregnancy != 1</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - pregnancy_end_date[previous pregnancy of the same person]</t>
+  </si>
+  <si>
+    <t>start_preg_period_pre_all</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 365</t>
+  </si>
+  <si>
+    <t>end_preg_period_pre_all</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 1</t>
+  </si>
+  <si>
+    <t>date when the period "12 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "12 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "9-12 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>end_preg_period_pre_3</t>
+  </si>
+  <si>
+    <t>start_preg_period_pre_3</t>
+  </si>
+  <si>
+    <t>date when the period "9-12 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 275</t>
+  </si>
+  <si>
+    <t>start_preg_period_pre_2</t>
+  </si>
+  <si>
+    <t>end_preg_period_pre_2</t>
+  </si>
+  <si>
+    <t>start_preg_period_pre_1</t>
+  </si>
+  <si>
+    <t>end_preg_period_pre_1</t>
+  </si>
+  <si>
+    <t>date when the period "6-9 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "6-9 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>start_preg_period_pre_4</t>
+  </si>
+  <si>
+    <t>end_preg_period_pre_4</t>
+  </si>
+  <si>
+    <t>date when the period "3-6 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "3-6 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "0-3 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "0-3 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 274</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 183</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 182</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 91</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 90</t>
+  </si>
+  <si>
+    <t>start_preg_period_during_1</t>
+  </si>
+  <si>
+    <t>end_preg_period_during_1</t>
+  </si>
+  <si>
+    <t>date when the period "First trimester of pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "First trimester of pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>min(pregnancy_start_date + 97, pregnancy_end_date)</t>
+  </si>
+  <si>
+    <t>start_preg_period_during_2</t>
+  </si>
+  <si>
+    <t>end_preg_period_during_2</t>
+  </si>
+  <si>
+    <t>min(pregnancy_start_date + 195, pregnancy_end_date)</t>
+  </si>
+  <si>
+    <t>min(pregnancy_start_date + 98, pregnancy_end_date)</t>
+  </si>
+  <si>
+    <t>if pregnancy ends before day 98, is this missing?</t>
+  </si>
+  <si>
+    <t>start_preg_period_during_3</t>
+  </si>
+  <si>
+    <t>end_preg_period_during_3</t>
+  </si>
+  <si>
+    <t>date when the period "Second trimester of pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "Second trimester of pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "Third trimester of pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "Third trimester of pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>min(pregnancy_start_date + 196, pregnancy_end_date)</t>
+  </si>
+  <si>
+    <t>if pregnancy ends before day 196, is this missing?</t>
+  </si>
+  <si>
+    <t>start_preg_period_after_1</t>
+  </si>
+  <si>
+    <t>end_preg_period_after_1</t>
+  </si>
+  <si>
+    <t>date when the period "0-3 months after pregnancy" starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period "0-3 months after pregnancy" ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>pregnancy_end_date + 1</t>
+  </si>
+  <si>
+    <t>pregnancy_end_date + 90</t>
+  </si>
+  <si>
+    <t>interval in days between the previous pregnancy and this one</t>
+  </si>
+  <si>
+    <t>1 = pregnancy with MS
 0 = otherwise</t>
   </si>
   <si>
-    <t>number of pregnancies with pregnancy_with_MS == 1</t>
-  </si>
-  <si>
-    <t>this is missing if has_MS_ever == 0, and 0 if has_MS_ever == 1 but there are no pregnancies with pregnancy_with_MS == 1</t>
-  </si>
-  <si>
-    <t>time_since_previous_pregnancy</t>
-  </si>
-  <si>
-    <t>time_since_previous_pregnancy_with_MS</t>
-  </si>
-  <si>
-    <t>has_previous_pregnancy</t>
-  </si>
-  <si>
-    <t>whether this pregnancy has a previous pregnancy of the same person in the study</t>
-  </si>
-  <si>
-    <t>has_previous_pregnancy_with_MS</t>
-  </si>
-  <si>
-    <t>missing if pregnancy_with_MS == 0</t>
-  </si>
-  <si>
-    <t>missing if has_previous_pregnancy_with_MS  != 1</t>
-  </si>
-  <si>
-    <t>missing if has_previous_pregnancy != 1</t>
-  </si>
-  <si>
-    <t>pregnancy_start_date - pregnancy_end_date[previous pregnancy of the same person]</t>
-  </si>
-  <si>
-    <t>interval in days between the orevious pregnancy and this one</t>
-  </si>
-  <si>
-    <t>interval in days between the previous pregnancy with MS and this one</t>
-  </si>
-  <si>
-    <t>whether this pregnancy has a previous pregnancy of the same person in the study with MS</t>
+    <t>MS_developed_during_pregnancy</t>
+  </si>
+  <si>
+    <t>1 = MS developed during pregnancy
+0 = otherwise</t>
+  </si>
+  <si>
+    <t>see table 5 page 12 of the SAP</t>
+  </si>
+  <si>
+    <t>Whether woman develops MS during or right after this pregnancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in DS with complete data this variable is 1 if
+pregnancy_with_MS_detail == "before  pregnancy"
+in THL and EFEMERIS this variable is 1 if
+pregnancy_with_MS_detail == "before  pregnancy" | pregnancy_with_MS_detail == "right before  pregnancy" (TO BE DECIDED: case when pregnancy_with_MS_detail == "during  pregnancy", and what about 'right after pregnancy'?)
+</t>
+  </si>
+  <si>
+    <t>pregnancy_with_MS_detail != "no" &amp; pregnancy_with_MS == 0 (check case right after pregnancy)</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>5 = More than 15 months
+4 = Between 12 and 15 months
+3 = Between 6 and 12 months 
+2 = Between 3 and 6 months
+1 = Less than 3 months</t>
+  </si>
+  <si>
+    <t>categories_time_since_previous_pregnancy</t>
+  </si>
+  <si>
+    <t>categories of interval between the previous pregnancy and this one</t>
+  </si>
+  <si>
+    <t>categorise time_since_previous_pregnancy</t>
+  </si>
+  <si>
+    <t>Whether woman has MS ever during the study period</t>
+  </si>
+  <si>
+    <t>date when MS is diagnosed</t>
+  </si>
+  <si>
+    <t>D4_DU_MS-COHORT</t>
+  </si>
+  <si>
+    <t>this is missing for all pregnancies where the linkage with D4_DU_MS-COHORT fails</t>
+  </si>
+  <si>
+    <t>See Figure 3 of the SAP. This is missing if has_MS_ever!= 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"long after pregnancy" = MS diagnosed after DU_pregnancy_study_exit_date
+"right after pregnancy" = MS diagnosed between pregnancy_end_date and DU_pregnancy_study_exit_date
+"during pregnancy" = MS diagnosed between pregnancy_start_date and pregnancy_end_date
+"right before pregnancy" = MS diagnosed between 3 months before pregnancy and pregnancy_start_date
+"recently before pregnancy" = MS diagnosed between DU_pregnancy_study_entry_date and 3 months before pregnancy 
+"long before pregnancy" = MS diagnosed before DU_pregnancy_study_entry_date
+</t>
+  </si>
+  <si>
+    <t>this needs to be adapted a bit across data sources??</t>
   </si>
 </sst>
 </file>
@@ -300,11 +488,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -394,7 +589,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,7 +610,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,150 +786,160 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -947,7 +1158,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -978,7 +1189,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6">
@@ -4008,13 +4219,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K977"/>
+  <dimension ref="A1:K976"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4022,9 +4233,9 @@
     <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.109375" style="41" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="35.77734375" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" style="41" customWidth="1"/>
     <col min="7" max="7" width="25.21875" customWidth="1"/>
     <col min="8" max="8" width="10.109375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
@@ -4112,7 +4323,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
       <c r="G4" s="35" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>23</v>
@@ -4127,7 +4338,7 @@
       <c r="D5" s="25"/>
       <c r="E5" s="26"/>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>23</v>
@@ -4146,7 +4357,7 @@
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="G6" s="51" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>23</v>
@@ -4165,7 +4376,7 @@
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
       <c r="G7" s="51" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>23</v>
@@ -4184,7 +4395,7 @@
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
       <c r="G8" s="51" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>23</v>
@@ -4195,10 +4406,10 @@
         <v>42</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H9" s="35" t="s">
         <v>23</v>
@@ -4209,15 +4420,18 @@
         <v>43</v>
       </c>
       <c r="B10" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>64</v>
+        <v>50</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="33" customHeight="1">
       <c r="A11" s="27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11" s="39" t="s">
         <v>31</v>
@@ -4227,14 +4441,18 @@
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
-      <c r="I11" s="18" t="s">
+      <c r="G11" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="35" t="s">
         <v>23</v>
       </c>
+      <c r="I11" s="18"/>
       <c r="K11" s="48"/>
     </row>
     <row r="12" spans="1:11" ht="34.799999999999997" customHeight="1">
       <c r="A12" s="27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B12" s="39" t="s">
         <v>32</v>
@@ -4244,218 +4462,580 @@
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
-      <c r="I12" s="18" t="s">
+      <c r="G12" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="35" t="s">
         <v>23</v>
       </c>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:11" ht="34.799999999999997" customHeight="1">
       <c r="A13" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="42" t="s">
-        <v>53</v>
+      <c r="B13" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
       </c>
       <c r="I13" s="42"/>
     </row>
-    <row r="14" spans="1:11" ht="34.799999999999997" customHeight="1">
+    <row r="14" spans="1:11" ht="28.8">
       <c r="A14" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E14" s="46"/>
       <c r="I14" s="42" t="s">
         <v>23</v>
       </c>
       <c r="K14" s="42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="158.4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="216">
       <c r="A15" s="44" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="49" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="E15" s="46"/>
-      <c r="F15" t="s">
-        <v>62</v>
+      <c r="F15" s="41" t="s">
+        <v>142</v>
       </c>
       <c r="I15" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="48"/>
-    </row>
-    <row r="16" spans="1:11" ht="43.2">
+      <c r="K15" s="60" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="144">
       <c r="A16" s="44" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B16" s="45" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="52" t="s">
-        <v>71</v>
+        <v>60</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>126</v>
       </c>
       <c r="E16" s="46"/>
-      <c r="I16" s="42"/>
-      <c r="K16" s="48"/>
-    </row>
-    <row r="17" spans="1:11" ht="34.799999999999997" customHeight="1">
-      <c r="A17" s="43" t="s">
-        <v>47</v>
+      <c r="I16" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="55" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="28.8">
+      <c r="A17" s="44" t="s">
+        <v>127</v>
       </c>
       <c r="B17" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="46"/>
+      <c r="D17" s="56" t="s">
+        <v>128</v>
+      </c>
       <c r="E17" s="46"/>
       <c r="I17" s="42" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="81" customHeight="1">
+      <c r="K17" s="57" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="34.799999999999997" customHeight="1">
       <c r="A18" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="I18" s="42" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="81" customHeight="1">
       <c r="A19" s="43" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C19" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="48"/>
-      <c r="I19" s="53" t="s">
+      <c r="F19" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="52" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45" customHeight="1">
+    <row r="20" spans="1:11" ht="81" customHeight="1">
       <c r="A20" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="45" customHeight="1">
+      <c r="A21" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="72">
+      <c r="A22" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="28.8">
+      <c r="A23" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="41" t="s">
+    </row>
+    <row r="24" spans="1:11" ht="28.8">
+      <c r="A24" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" t="s">
+    </row>
+    <row r="25" spans="1:11" ht="28.8">
+      <c r="A25" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="53" t="s">
+      <c r="B25" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="28.8" customHeight="1">
-      <c r="A21" s="43" t="s">
+      <c r="K25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28.8">
+      <c r="A26" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="28.8">
+      <c r="A27" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I27" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="28.8">
+      <c r="A28" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="28.8">
+      <c r="A29" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I29" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="28.8">
+      <c r="A30" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I30" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="28.8">
+      <c r="A31" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I31" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="28.8">
+      <c r="A32" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="28.8">
+      <c r="A33" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="I33" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="54" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="28.8">
+      <c r="A34" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="28.8">
+      <c r="A35" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="I35" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="54" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="28.8">
+      <c r="A36" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="I36" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="28.8">
+      <c r="A37" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I37" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="28.8">
+      <c r="A38" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I38" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="28.8">
+      <c r="A39" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I39" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="28.8">
+      <c r="A40" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="54" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="53" t="s">
+      <c r="C40" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I40" s="53" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="38.4" customHeight="1">
-      <c r="A22" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="I22" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+      <c r="K40" s="43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="52" ht="14.4"/>
+    <row r="53" ht="14.4"/>
     <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1"/>
     <row r="56" ht="15.75" customHeight="1"/>
@@ -5379,7 +5959,6 @@
     <row r="974" ht="15.75" customHeight="1"/>
     <row r="975" ht="15.75" customHeight="1"/>
     <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>